<commit_message>
All updates for draft 20180205.
</commit_message>
<xml_diff>
--- a/tables_1_2.xlsx
+++ b/tables_1_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Period SRX" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Sweden</t>
   </si>
@@ -90,52 +90,40 @@
     <t>Std. Dev.</t>
   </si>
   <si>
-    <t>1850-1966</t>
-  </si>
-  <si>
-    <t>1921-1964</t>
-  </si>
-  <si>
-    <t>1872-1964</t>
-  </si>
-  <si>
-    <t>1947-1964</t>
-  </si>
-  <si>
     <t>1959-1964</t>
   </si>
   <si>
-    <t>1933-1965</t>
-  </si>
-  <si>
     <t>Years Without Cross</t>
   </si>
   <si>
-    <t>Cohorts Without Cross</t>
-  </si>
-  <si>
-    <t>1956-1963</t>
-  </si>
-  <si>
-    <t>1954-1963</t>
-  </si>
-  <si>
-    <t>1950-1965</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>Available Cohorts</t>
   </si>
   <si>
-    <t>Not Applicable</t>
-  </si>
-  <si>
     <t>1992-2007</t>
   </si>
   <si>
     <t>1873-1879, 1883-1894</t>
+  </si>
+  <si>
+    <t>1850-1964</t>
+  </si>
+  <si>
+    <t>1933-1964</t>
+  </si>
+  <si>
+    <t>1850-1949</t>
+  </si>
+  <si>
+    <t>1921-1955</t>
+  </si>
+  <si>
+    <t>1947-1954</t>
+  </si>
+  <si>
+    <t>1872-1955</t>
   </si>
 </sst>
 </file>
@@ -143,9 +131,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +148,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,15 +185,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:G10"/>
     </sheetView>
   </sheetViews>
@@ -514,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -537,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -560,7 +557,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>48</v>
@@ -580,10 +577,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>45</v>
@@ -606,7 +603,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>19</v>
@@ -629,7 +626,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>47</v>
@@ -652,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>29</v>
@@ -675,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -698,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>44</v>
@@ -724,219 +721,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>9</v>
-      </c>
-      <c r="E3">
         <v>64</v>
       </c>
+      <c r="E3" s="2">
+        <v>47.833959999999998</v>
+      </c>
       <c r="F3" s="2">
-        <v>47.723480000000002</v>
-      </c>
-      <c r="G3" s="2">
-        <v>11.6199014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11.623626399999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>43</v>
       </c>
       <c r="D4">
-        <v>43</v>
-      </c>
-      <c r="E4">
         <v>61</v>
       </c>
+      <c r="E4" s="2">
+        <v>51.68571</v>
+      </c>
       <c r="F4" s="2">
-        <v>51.68571</v>
-      </c>
-      <c r="G4" s="2">
         <v>4.5682498999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>19</v>
-      </c>
-      <c r="E5">
         <v>63</v>
       </c>
+      <c r="E5" s="2">
+        <v>42.940480000000001</v>
+      </c>
       <c r="F5" s="2">
-        <v>42.869050000000001</v>
-      </c>
-      <c r="G5" s="2">
-        <v>14.009273800000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14.0501264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
       </c>
       <c r="D6">
-        <v>55</v>
-      </c>
-      <c r="E6">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="E6" s="2">
+        <v>56.625</v>
       </c>
       <c r="F6" s="2">
-        <v>56.142859999999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.069045</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.3024701999999999</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2">
         <v>32</v>
       </c>
-      <c r="D7">
-        <v>31</v>
-      </c>
-      <c r="E7">
-        <v>33</v>
-      </c>
       <c r="F7" s="2">
-        <v>32</v>
-      </c>
-      <c r="G7" s="2">
         <v>0.63245549999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K7" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2">
+        <v>51.58</v>
+      </c>
+      <c r="F8" s="2">
+        <v>11.1075368</v>
+      </c>
+      <c r="K8" s="5">
         <v>31</v>
       </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2">
-        <v>51.48</v>
-      </c>
-      <c r="G8" s="2">
-        <v>11.1423117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1965</v>
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>42</v>
       </c>
       <c r="D9">
-        <v>42</v>
-      </c>
-      <c r="E9">
         <v>51</v>
       </c>
+      <c r="E9" s="2">
+        <v>45.53125</v>
+      </c>
       <c r="F9" s="2">
-        <v>45.5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2.0790817000000001</v>
+        <v>1.9672213000000001</v>
+      </c>
+      <c r="K9" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>